<commit_message>
lagt til stst på urgent
</commit_message>
<xml_diff>
--- a/ExampleIG/output/CodeSystem-hn-kodeverk-varsling.codesystem.xlsx
+++ b/ExampleIG/output/CodeSystem-hn-kodeverk-varsling.codesystem.xlsx
@@ -36,7 +36,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.3.0</t>
+    <t>1.3.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -66,7 +66,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-29T13:18:42+02:00</t>
+    <t>2025-10-01T13:36:52+02:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>